<commit_message>
Added new model selection experiments
</commit_message>
<xml_diff>
--- a/docs/Experiment 1 - Usokin/Experiment 1B Results.xlsx
+++ b/docs/Experiment 1 - Usokin/Experiment 1B Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="100g, Scaled, 1 Layer" sheetId="2" r:id="rId1"/>
@@ -1583,11 +1583,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1595,8 +1595,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1604,17 +1613,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="60">
@@ -1699,6 +1699,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1748,11 +1749,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2021031400"/>
-        <c:axId val="2021032072"/>
+        <c:axId val="2085290232"/>
+        <c:axId val="2085293176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2021031400"/>
+        <c:axId val="2085290232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1761,7 +1762,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2021032072"/>
+        <c:crossAx val="2085293176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1769,7 +1770,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2021032072"/>
+        <c:axId val="2085293176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1780,13 +1781,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2021031400"/>
+        <c:crossAx val="2085290232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2426,11 +2428,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2029801848"/>
-        <c:axId val="2094159208"/>
+        <c:axId val="2084692488"/>
+        <c:axId val="2084689496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2029801848"/>
+        <c:axId val="2084692488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2439,7 +2441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2094159208"/>
+        <c:crossAx val="2084689496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2448,7 +2450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2094159208"/>
+        <c:axId val="2084689496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100.0"/>
@@ -2460,7 +2462,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2029801848"/>
+        <c:crossAx val="2084692488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3097,11 +3099,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2091528776"/>
-        <c:axId val="2091531752"/>
+        <c:axId val="2084660584"/>
+        <c:axId val="2084657592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2091528776"/>
+        <c:axId val="2084660584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3110,7 +3112,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091531752"/>
+        <c:crossAx val="2084657592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3119,7 +3121,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091531752"/>
+        <c:axId val="2084657592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80.0"/>
@@ -3131,7 +3133,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091528776"/>
+        <c:crossAx val="2084660584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3785,11 +3787,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2091745144"/>
-        <c:axId val="2090951512"/>
+        <c:axId val="2084628424"/>
+        <c:axId val="2084625432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2091745144"/>
+        <c:axId val="2084628424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3798,7 +3800,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090951512"/>
+        <c:crossAx val="2084625432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3808,7 +3810,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090951512"/>
+        <c:axId val="2084625432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8.0"/>
@@ -3820,7 +3822,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091745144"/>
+        <c:crossAx val="2084628424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4474,11 +4476,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2019855384"/>
-        <c:axId val="2091767976"/>
+        <c:axId val="2084596328"/>
+        <c:axId val="2084593336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2019855384"/>
+        <c:axId val="2084596328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4487,7 +4489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091767976"/>
+        <c:crossAx val="2084593336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4496,7 +4498,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091767976"/>
+        <c:axId val="2084593336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80.0"/>
@@ -4508,7 +4510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2019855384"/>
+        <c:crossAx val="2084596328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5157,11 +5159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2030009048"/>
-        <c:axId val="2029976920"/>
+        <c:axId val="2086813544"/>
+        <c:axId val="2086816520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2030009048"/>
+        <c:axId val="2086813544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5170,7 +5172,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2029976920"/>
+        <c:crossAx val="2086816520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5178,7 +5180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2029976920"/>
+        <c:axId val="2086816520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80.0"/>
@@ -5190,7 +5192,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2030009048"/>
+        <c:crossAx val="2086813544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5271,11 +5273,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2021014488"/>
-        <c:axId val="2021102024"/>
+        <c:axId val="2085358184"/>
+        <c:axId val="2085361128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2021014488"/>
+        <c:axId val="2085358184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5284,7 +5286,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2021102024"/>
+        <c:crossAx val="2085361128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5292,7 +5294,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2021102024"/>
+        <c:axId val="2085361128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5303,7 +5305,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2021014488"/>
+        <c:crossAx val="2085358184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5715,11 +5717,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132983160"/>
-        <c:axId val="2089904232"/>
+        <c:axId val="2085388248"/>
+        <c:axId val="2085391192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132983160"/>
+        <c:axId val="2085388248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5728,7 +5730,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089904232"/>
+        <c:crossAx val="2085391192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5736,7 +5738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089904232"/>
+        <c:axId val="2085391192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80.0"/>
@@ -5748,7 +5750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132983160"/>
+        <c:crossAx val="2085388248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6159,11 +6161,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2090530392"/>
-        <c:axId val="2132997304"/>
+        <c:axId val="2085424584"/>
+        <c:axId val="2085427560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2090530392"/>
+        <c:axId val="2085424584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6172,7 +6174,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132997304"/>
+        <c:crossAx val="2085427560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6180,7 +6182,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132997304"/>
+        <c:axId val="2085427560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -6192,7 +6194,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090530392"/>
+        <c:crossAx val="2085424584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6595,11 +6597,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132881464"/>
-        <c:axId val="2090119064"/>
+        <c:axId val="2085456200"/>
+        <c:axId val="2085459176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132881464"/>
+        <c:axId val="2085456200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6608,7 +6610,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090119064"/>
+        <c:crossAx val="2085459176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6616,7 +6618,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090119064"/>
+        <c:axId val="2085459176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80.0"/>
@@ -6628,7 +6630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132881464"/>
+        <c:crossAx val="2085456200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7353,11 +7355,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132971320"/>
-        <c:axId val="2132852904"/>
+        <c:axId val="2085490920"/>
+        <c:axId val="2085493896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132971320"/>
+        <c:axId val="2085490920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7366,7 +7368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132852904"/>
+        <c:crossAx val="2085493896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7374,7 +7376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132852904"/>
+        <c:axId val="2085493896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -7386,7 +7388,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132971320"/>
+        <c:crossAx val="2085490920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8112,11 +8114,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2090649768"/>
-        <c:axId val="2090666872"/>
+        <c:axId val="2085522920"/>
+        <c:axId val="2085525896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2090649768"/>
+        <c:axId val="2085522920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8125,7 +8127,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090666872"/>
+        <c:crossAx val="2085525896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8133,7 +8135,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090666872"/>
+        <c:axId val="2085525896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100.0"/>
@@ -8145,7 +8147,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090649768"/>
+        <c:crossAx val="2085522920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8866,11 +8868,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2090655544"/>
-        <c:axId val="2090658520"/>
+        <c:axId val="2085552248"/>
+        <c:axId val="2085555224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2090655544"/>
+        <c:axId val="2085552248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8879,7 +8881,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090658520"/>
+        <c:crossAx val="2085555224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8887,7 +8889,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090658520"/>
+        <c:axId val="2085555224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80.0"/>
@@ -8899,7 +8901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090655544"/>
+        <c:crossAx val="2085552248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9541,11 +9543,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2091945656"/>
-        <c:axId val="2019854584"/>
+        <c:axId val="2085589000"/>
+        <c:axId val="2085591976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2091945656"/>
+        <c:axId val="2085589000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9554,7 +9556,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2019854584"/>
+        <c:crossAx val="2085591976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9563,7 +9565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2019854584"/>
+        <c:axId val="2085591976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -9575,7 +9577,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091945656"/>
+        <c:crossAx val="2085589000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10579,11 +10581,13 @@
   <dimension ref="A1:T52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12284,8 +12288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL108"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12314,50 +12318,50 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="I1" s="27" t="str">
+      <c r="I1" s="18" t="str">
         <f>G3</f>
         <v>50_UsokinVAE_FINAL</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Y1" s="23" t="str">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Y1" s="26" t="str">
         <f>G4</f>
         <v>53_UsokinVAE_FINAL</v>
       </c>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AO1" s="23" t="str">
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
+      <c r="AO1" s="26" t="str">
         <f>G5</f>
         <v>52_UsokinVAE_FINAL</v>
       </c>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="24"/>
-      <c r="AT1" s="24"/>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24"/>
-      <c r="BE1" s="23" t="str">
+      <c r="AP1" s="27"/>
+      <c r="AQ1" s="27"/>
+      <c r="AR1" s="27"/>
+      <c r="AS1" s="27"/>
+      <c r="AT1" s="27"/>
+      <c r="AU1" s="27"/>
+      <c r="AV1" s="27"/>
+      <c r="BE1" s="26" t="str">
         <f>G6</f>
         <v>51_UsokinVAE_FINAL</v>
       </c>
-      <c r="BF1" s="24"/>
-      <c r="BG1" s="24"/>
-      <c r="BH1" s="24"/>
-      <c r="BI1" s="24"/>
-      <c r="BJ1" s="24"/>
-      <c r="BK1" s="24"/>
-      <c r="BL1" s="24"/>
+      <c r="BF1" s="27"/>
+      <c r="BG1" s="27"/>
+      <c r="BH1" s="27"/>
+      <c r="BI1" s="27"/>
+      <c r="BJ1" s="27"/>
+      <c r="BK1" s="27"/>
+      <c r="BL1" s="27"/>
     </row>
     <row r="2" spans="1:64" ht="16" customHeight="1" thickTop="1">
       <c r="A2" s="3" t="s">
@@ -12386,49 +12390,49 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
       <c r="Y2" s="20" t="s">
         <v>129</v>
       </c>
       <c r="Z2" s="21"/>
       <c r="AA2" s="21"/>
-      <c r="AB2" s="22" t="s">
+      <c r="AB2" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="28"/>
       <c r="AO2" s="20" t="s">
         <v>129</v>
       </c>
       <c r="AP2" s="21"/>
       <c r="AQ2" s="21"/>
-      <c r="AR2" s="22" t="s">
+      <c r="AR2" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="22"/>
-      <c r="AU2" s="22"/>
-      <c r="AV2" s="22"/>
+      <c r="AS2" s="28"/>
+      <c r="AT2" s="28"/>
+      <c r="AU2" s="28"/>
+      <c r="AV2" s="28"/>
       <c r="BE2" s="20" t="s">
         <v>129</v>
       </c>
       <c r="BF2" s="21"/>
       <c r="BG2" s="21"/>
-      <c r="BH2" s="22" t="s">
+      <c r="BH2" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
+      <c r="BI2" s="28"/>
+      <c r="BJ2" s="28"/>
+      <c r="BK2" s="28"/>
+      <c r="BL2" s="28"/>
     </row>
     <row r="3" spans="1:64" ht="15" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -12457,49 +12461,49 @@
       </c>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
       <c r="Y3" s="20" t="s">
         <v>179</v>
       </c>
       <c r="Z3" s="21"/>
       <c r="AA3" s="21"/>
-      <c r="AB3" s="22" t="s">
+      <c r="AB3" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="AC3" s="22"/>
-      <c r="AD3" s="22"/>
-      <c r="AE3" s="22"/>
-      <c r="AF3" s="22"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="28"/>
       <c r="AO3" s="20" t="s">
         <v>179</v>
       </c>
       <c r="AP3" s="21"/>
       <c r="AQ3" s="21"/>
-      <c r="AR3" s="22" t="s">
+      <c r="AR3" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="AS3" s="22"/>
-      <c r="AT3" s="22"/>
-      <c r="AU3" s="22"/>
-      <c r="AV3" s="22"/>
+      <c r="AS3" s="28"/>
+      <c r="AT3" s="28"/>
+      <c r="AU3" s="28"/>
+      <c r="AV3" s="28"/>
       <c r="BE3" s="20" t="s">
         <v>179</v>
       </c>
       <c r="BF3" s="21"/>
       <c r="BG3" s="21"/>
-      <c r="BH3" s="22" t="s">
+      <c r="BH3" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="BI3" s="22"/>
-      <c r="BJ3" s="22"/>
-      <c r="BK3" s="22"/>
-      <c r="BL3" s="22"/>
+      <c r="BI3" s="28"/>
+      <c r="BJ3" s="28"/>
+      <c r="BK3" s="28"/>
+      <c r="BL3" s="28"/>
     </row>
     <row r="4" spans="1:64" ht="15" customHeight="1">
       <c r="A4" s="4" t="s">
@@ -12528,49 +12532,49 @@
       </c>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
-      <c r="L4" s="22">
+      <c r="L4" s="28">
         <v>50</v>
       </c>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
       <c r="Y4" s="20" t="s">
         <v>180</v>
       </c>
       <c r="Z4" s="21"/>
       <c r="AA4" s="21"/>
-      <c r="AB4" s="22">
+      <c r="AB4" s="28">
         <v>11</v>
       </c>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="28"/>
       <c r="AO4" s="20" t="s">
         <v>180</v>
       </c>
       <c r="AP4" s="21"/>
       <c r="AQ4" s="21"/>
-      <c r="AR4" s="22">
+      <c r="AR4" s="28">
         <v>25</v>
       </c>
-      <c r="AS4" s="22"/>
-      <c r="AT4" s="22"/>
-      <c r="AU4" s="22"/>
-      <c r="AV4" s="22"/>
+      <c r="AS4" s="28"/>
+      <c r="AT4" s="28"/>
+      <c r="AU4" s="28"/>
+      <c r="AV4" s="28"/>
       <c r="BE4" s="20" t="s">
         <v>180</v>
       </c>
       <c r="BF4" s="21"/>
       <c r="BG4" s="21"/>
-      <c r="BH4" s="22">
+      <c r="BH4" s="28">
         <v>25</v>
       </c>
-      <c r="BI4" s="22"/>
-      <c r="BJ4" s="22"/>
-      <c r="BK4" s="22"/>
-      <c r="BL4" s="22"/>
+      <c r="BI4" s="28"/>
+      <c r="BJ4" s="28"/>
+      <c r="BK4" s="28"/>
+      <c r="BL4" s="28"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1">
       <c r="A5" s="4" t="s">
@@ -12599,49 +12603,49 @@
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
-      <c r="L5" s="22" t="s">
+      <c r="L5" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
       <c r="Y5" s="20" t="s">
         <v>131</v>
       </c>
       <c r="Z5" s="21"/>
       <c r="AA5" s="21"/>
-      <c r="AB5" s="22" t="s">
+      <c r="AB5" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="22"/>
-      <c r="AE5" s="22"/>
-      <c r="AF5" s="22"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="28"/>
+      <c r="AE5" s="28"/>
+      <c r="AF5" s="28"/>
       <c r="AO5" s="20" t="s">
         <v>131</v>
       </c>
       <c r="AP5" s="21"/>
       <c r="AQ5" s="21"/>
-      <c r="AR5" s="22" t="s">
+      <c r="AR5" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="AS5" s="22"/>
-      <c r="AT5" s="22"/>
-      <c r="AU5" s="22"/>
-      <c r="AV5" s="22"/>
+      <c r="AS5" s="28"/>
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="28"/>
+      <c r="AV5" s="28"/>
       <c r="BE5" s="20" t="s">
         <v>131</v>
       </c>
       <c r="BF5" s="21"/>
       <c r="BG5" s="21"/>
-      <c r="BH5" s="22" t="s">
+      <c r="BH5" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="BI5" s="22"/>
-      <c r="BJ5" s="22"/>
-      <c r="BK5" s="22"/>
-      <c r="BL5" s="22"/>
+      <c r="BI5" s="28"/>
+      <c r="BJ5" s="28"/>
+      <c r="BK5" s="28"/>
+      <c r="BL5" s="28"/>
     </row>
     <row r="6" spans="1:64" ht="16" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -12670,49 +12674,49 @@
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="21"/>
-      <c r="L6" s="22">
+      <c r="L6" s="28">
         <v>25</v>
       </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
       <c r="Y6" s="20" t="s">
         <v>132</v>
       </c>
       <c r="Z6" s="21"/>
       <c r="AA6" s="21"/>
-      <c r="AB6" s="22">
+      <c r="AB6" s="28">
         <v>25</v>
       </c>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="22"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
       <c r="AO6" s="20" t="s">
         <v>132</v>
       </c>
       <c r="AP6" s="21"/>
       <c r="AQ6" s="21"/>
-      <c r="AR6" s="22">
+      <c r="AR6" s="28">
         <v>10</v>
       </c>
-      <c r="AS6" s="22"/>
-      <c r="AT6" s="22"/>
-      <c r="AU6" s="22"/>
-      <c r="AV6" s="22"/>
+      <c r="AS6" s="28"/>
+      <c r="AT6" s="28"/>
+      <c r="AU6" s="28"/>
+      <c r="AV6" s="28"/>
       <c r="BE6" s="20" t="s">
         <v>132</v>
       </c>
       <c r="BF6" s="21"/>
       <c r="BG6" s="21"/>
-      <c r="BH6" s="22">
+      <c r="BH6" s="28">
         <v>10</v>
       </c>
-      <c r="BI6" s="22"/>
-      <c r="BJ6" s="22"/>
-      <c r="BK6" s="22"/>
-      <c r="BL6" s="22"/>
+      <c r="BI6" s="28"/>
+      <c r="BJ6" s="28"/>
+      <c r="BK6" s="28"/>
+      <c r="BL6" s="28"/>
     </row>
     <row r="7" spans="1:64">
       <c r="A7" s="5" t="s">
@@ -12734,46 +12738,46 @@
         <v>115.108644</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Y7" s="18" t="s">
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Y7" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="Z7" s="19"/>
-      <c r="AA7" s="19"/>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="19"/>
-      <c r="AE7" s="19"/>
-      <c r="AF7" s="19"/>
-      <c r="AO7" s="18" t="s">
+      <c r="Z7" s="23"/>
+      <c r="AA7" s="23"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="23"/>
+      <c r="AE7" s="23"/>
+      <c r="AF7" s="23"/>
+      <c r="AO7" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="AP7" s="19"/>
-      <c r="AQ7" s="19"/>
-      <c r="AR7" s="19"/>
-      <c r="AS7" s="19"/>
-      <c r="AT7" s="19"/>
-      <c r="AU7" s="19"/>
-      <c r="AV7" s="19"/>
-      <c r="BE7" s="18" t="s">
+      <c r="AP7" s="23"/>
+      <c r="AQ7" s="23"/>
+      <c r="AR7" s="23"/>
+      <c r="AS7" s="23"/>
+      <c r="AT7" s="23"/>
+      <c r="AU7" s="23"/>
+      <c r="AV7" s="23"/>
+      <c r="BE7" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="BF7" s="19"/>
-      <c r="BG7" s="19"/>
-      <c r="BH7" s="19"/>
-      <c r="BI7" s="19"/>
-      <c r="BJ7" s="19"/>
-      <c r="BK7" s="19"/>
-      <c r="BL7" s="19"/>
+      <c r="BF7" s="23"/>
+      <c r="BG7" s="23"/>
+      <c r="BH7" s="23"/>
+      <c r="BI7" s="23"/>
+      <c r="BJ7" s="23"/>
+      <c r="BK7" s="23"/>
+      <c r="BL7" s="23"/>
     </row>
     <row r="8" spans="1:64">
       <c r="A8" s="5" t="s">
@@ -21615,11 +21619,34 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="AO7:AV7"/>
+    <mergeCell ref="BE7:BL7"/>
+    <mergeCell ref="BE4:BG4"/>
+    <mergeCell ref="BH4:BL4"/>
+    <mergeCell ref="BE5:BG5"/>
+    <mergeCell ref="BH5:BL5"/>
+    <mergeCell ref="BE6:BG6"/>
+    <mergeCell ref="BH6:BL6"/>
+    <mergeCell ref="AO4:AQ4"/>
+    <mergeCell ref="AR4:AV4"/>
+    <mergeCell ref="AR5:AV5"/>
+    <mergeCell ref="AR6:AV6"/>
+    <mergeCell ref="BE1:BL1"/>
+    <mergeCell ref="BE2:BG2"/>
+    <mergeCell ref="BH2:BL2"/>
+    <mergeCell ref="BE3:BG3"/>
+    <mergeCell ref="BH3:BL3"/>
+    <mergeCell ref="AO1:AV1"/>
+    <mergeCell ref="AO2:AQ2"/>
+    <mergeCell ref="AR2:AV2"/>
+    <mergeCell ref="AO3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="AB5:AF5"/>
+    <mergeCell ref="Y6:AA6"/>
+    <mergeCell ref="AB6:AF6"/>
+    <mergeCell ref="AO5:AQ5"/>
+    <mergeCell ref="AO6:AQ6"/>
     <mergeCell ref="Y7:AF7"/>
     <mergeCell ref="I7:P7"/>
     <mergeCell ref="Y1:AF1"/>
@@ -21636,34 +21663,11 @@
     <mergeCell ref="L5:P5"/>
     <mergeCell ref="L6:P6"/>
     <mergeCell ref="I5:K5"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AB5:AF5"/>
-    <mergeCell ref="Y6:AA6"/>
-    <mergeCell ref="AB6:AF6"/>
-    <mergeCell ref="AO5:AQ5"/>
-    <mergeCell ref="AO6:AQ6"/>
-    <mergeCell ref="AO1:AV1"/>
-    <mergeCell ref="AO2:AQ2"/>
-    <mergeCell ref="AR2:AV2"/>
-    <mergeCell ref="AO3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="BE1:BL1"/>
-    <mergeCell ref="BE2:BG2"/>
-    <mergeCell ref="BH2:BL2"/>
-    <mergeCell ref="BE3:BG3"/>
-    <mergeCell ref="BH3:BL3"/>
-    <mergeCell ref="AO7:AV7"/>
-    <mergeCell ref="BE7:BL7"/>
-    <mergeCell ref="BE4:BG4"/>
-    <mergeCell ref="BH4:BL4"/>
-    <mergeCell ref="BE5:BG5"/>
-    <mergeCell ref="BH5:BL5"/>
-    <mergeCell ref="BE6:BG6"/>
-    <mergeCell ref="BH6:BL6"/>
-    <mergeCell ref="AO4:AQ4"/>
-    <mergeCell ref="AR4:AV4"/>
-    <mergeCell ref="AR5:AV5"/>
-    <mergeCell ref="AR6:AV6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -21686,7 +21690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>

</xml_diff>